<commit_message>
Adder - front panel PCB
</commit_message>
<xml_diff>
--- a/modules/Adder/panel-positions.xlsx
+++ b/modules/Adder/panel-positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Adder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AE4FBC3-1093-4318-AD7D-7EEB31A55E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05C618F-C8A1-4356-841C-5F8448B3C6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="1710" windowWidth="19380" windowHeight="11835" xr2:uid="{B82FF206-EC2D-4DC4-8A75-844E2FF9ECB9}"/>
+    <workbookView xWindow="7425" yWindow="1470" windowWidth="19380" windowHeight="11835" xr2:uid="{B82FF206-EC2D-4DC4-8A75-844E2FF9ECB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>top jack</t>
   </si>
@@ -56,15 +56,6 @@
     <t>bottom jack</t>
   </si>
   <si>
-    <t>jack X</t>
-  </si>
-  <si>
-    <t>LED X</t>
-  </si>
-  <si>
-    <t>4.3/4.4</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -93,6 +84,9 @@
   </si>
   <si>
     <t>J8</t>
+  </si>
+  <si>
+    <t>rects</t>
   </si>
 </sst>
 </file>
@@ -444,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7AB207-DE9C-4076-9584-E5152570F1DF}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,139 +457,375 @@
         <v>6</v>
       </c>
       <c r="E1">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65.227999999999994</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>65.227999999999994</v>
+      </c>
+      <c r="J1">
+        <f>L1+K1/2</f>
+        <v>25.228000000000002</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>22.228000000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>0.42500000000000027</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>E3-E1</f>
+        <v>9.3980000000000103</v>
+      </c>
+      <c r="I2">
+        <v>10.794999999999987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>0.37000000000000011</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>74.626000000000005</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <f>H1+I2</f>
+        <v>76.022999999999982</v>
+      </c>
+      <c r="J3">
+        <f>J1+I2</f>
+        <v>36.022999999999989</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <f>J3-K3/2</f>
+        <v>33.022999999999989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>0.37999999999999989</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>E5-E3</f>
+        <v>9.652000000000001</v>
+      </c>
+      <c r="I4">
+        <v>10.794999999999987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.64999999999999991</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>84.278000000000006</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <f>H3+I4</f>
+        <v>86.817999999999969</v>
+      </c>
+      <c r="J5">
+        <f>J3+I4</f>
+        <v>46.817999999999977</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f>J5-K5/2</f>
+        <v>43.817999999999977</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>E7-E5</f>
+        <v>10.794999999999987</v>
+      </c>
+      <c r="I6">
+        <v>9.3980000000000103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>95.072999999999993</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <f>H5+I6</f>
+        <v>96.21599999999998</v>
+      </c>
+      <c r="J7">
+        <f>J5+I6</f>
+        <v>56.215999999999987</v>
+      </c>
+      <c r="K7">
+        <v>2.75</v>
+      </c>
+      <c r="L7">
+        <f>J7-K7/2</f>
+        <v>54.840999999999987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <f>$B$1</f>
         <v>1.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>E9-E7</f>
+        <v>10.795000000000002</v>
+      </c>
+      <c r="I8">
+        <v>9.652000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <f>B8+$B$2</f>
         <v>2.0750000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>105.86799999999999</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <f>H7+I8</f>
+        <v>105.86799999999998</v>
+      </c>
+      <c r="J9">
+        <f>J7+I8</f>
+        <v>65.867999999999995</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f>J9-K9/2</f>
+        <v>62.867999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f>B9+$B$2</f>
         <v>2.5000000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>E11-E9</f>
+        <v>16.510000000000005</v>
+      </c>
+      <c r="I10">
+        <v>16.510000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>B10+$B$3</f>
         <v>2.8700000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>122.378</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <f>H9+I10</f>
+        <v>122.37799999999999</v>
+      </c>
+      <c r="J11">
+        <f>J9+I10</f>
+        <v>82.378</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <f>J11-K11/2</f>
+        <v>79.378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <f>B11+$B$4</f>
         <v>3.2500000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>E13-E11</f>
+        <v>9.3980000000000103</v>
+      </c>
+      <c r="I12">
+        <v>10.794999999999987</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <f>B12+$B$5</f>
         <v>3.9000000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>131.77600000000001</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <f>H11+I12</f>
+        <v>133.17299999999997</v>
+      </c>
+      <c r="J13">
+        <f>J11+I12</f>
+        <v>93.172999999999988</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f>J13-K13/2</f>
+        <v>90.172999999999988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <f>B13+$B$2</f>
         <v>4.3250000000000011</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f>E15-E13</f>
+        <v>9.6519999999999868</v>
+      </c>
+      <c r="I14">
+        <v>10.794999999999987</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <f>B14+$B$2</f>
         <v>4.7500000000000018</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>141.428</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <f>H13+I14</f>
+        <v>143.96799999999996</v>
+      </c>
+      <c r="J15">
+        <f>J13+I14</f>
+        <v>103.96799999999998</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <f>J15-K15/2</f>
+        <v>100.96799999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <f>B15+$B$3</f>
         <v>5.1200000000000019</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>E17-E15</f>
+        <v>10.795000000000016</v>
+      </c>
+      <c r="I16">
+        <v>9.3980000000000103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <f>B16+$B$4</f>
@@ -604,6 +834,78 @@
       <c r="C17" t="b">
         <f>B17=B6</f>
         <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>152.22300000000001</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <f>H15+I16</f>
+        <v>153.36599999999999</v>
+      </c>
+      <c r="J17">
+        <f>J15+I16</f>
+        <v>113.36599999999999</v>
+      </c>
+      <c r="K17">
+        <v>2.75</v>
+      </c>
+      <c r="L17">
+        <f>J17-K17/2</f>
+        <v>111.99099999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f>E19-E17</f>
+        <v>10.794999999999987</v>
+      </c>
+      <c r="I18">
+        <v>9.652000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>163.018</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <f>H17+I18</f>
+        <v>163.01799999999997</v>
+      </c>
+      <c r="J19">
+        <f>J17+I18</f>
+        <v>123.01799999999999</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <f>J19-K19/2</f>
+        <v>120.01799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21">
+        <v>39.918999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>97.069000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>